<commit_message>
change Hight Quality Course Program
</commit_message>
<xml_diff>
--- a/High-Quality-Course-Program-July-2015.xlsx
+++ b/High-Quality-Course-Program-July-2015.xlsx
@@ -183,7 +183,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\ mmm"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,6 +210,15 @@
       <scheme val="major"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri Light"/>
@@ -244,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -277,6 +286,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -709,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -941,7 +960,7 @@
       <c r="F9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="13">
         <f>Table1[[#This Row],[Date]]+7</f>
         <v>42207</v>
       </c>
@@ -966,7 +985,7 @@
       <c r="F10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="13">
         <f>Table1[[#This Row],[Date]]+7</f>
         <v>42207</v>
       </c>
@@ -1046,76 +1065,76 @@
         <v>42212</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="12">
+      <c r="C14" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="17">
         <v>42206</v>
       </c>
-      <c r="E14" s="11" t="str">
+      <c r="E14" s="16" t="str">
         <f>TEXT(Table1[[#This Row],[Date]],"dddd")</f>
         <v>Tuesday</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
+    <row r="15" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
         <v>8</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="3">
+      <c r="C15" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="8">
         <v>42207</v>
       </c>
-      <c r="E15" s="2" t="str">
+      <c r="E15" s="7" t="str">
         <f>TEXT(Table1[[#This Row],[Date]],"dddd")</f>
         <v>Wednesday</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="8">
         <f>Table1[[#This Row],[Date]]+7</f>
         <v>42214</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
+    <row r="16" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
         <v>8</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="3">
+      <c r="C16" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="8">
         <v>42207</v>
       </c>
-      <c r="E16" s="2" t="str">
+      <c r="E16" s="7" t="str">
         <f>TEXT(Table1[[#This Row],[Date]],"dddd")</f>
         <v>Wednesday</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="8">
         <f>Table1[[#This Row],[Date]]+7</f>
         <v>42214</v>
       </c>

</xml_diff>

<commit_message>
update program for course
</commit_message>
<xml_diff>
--- a/High-Quality-Course-Program-July-2015.xlsx
+++ b/High-Quality-Course-Program-July-2015.xlsx
@@ -729,7 +729,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="G11" sqref="G11:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1010,7 +1010,7 @@
       <c r="F11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="13">
         <f>Table1[[#This Row],[Date]]+7</f>
         <v>42208</v>
       </c>
@@ -1035,7 +1035,7 @@
       <c r="F12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="13">
         <f>Table1[[#This Row],[Date]]+7</f>
         <v>42208</v>
       </c>
@@ -1060,7 +1060,7 @@
       <c r="F13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="13">
         <f>Table1[[#This Row],[Date]]+7</f>
         <v>42212</v>
       </c>

</xml_diff>

<commit_message>
update program for HQC
</commit_message>
<xml_diff>
--- a/High-Quality-Course-Program-July-2015.xlsx
+++ b/High-Quality-Course-Program-July-2015.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3744" yWindow="0" windowWidth="22728" windowHeight="7296"/>
+    <workbookView xWindow="4680" yWindow="0" windowWidth="22728" windowHeight="7296"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="51">
   <si>
     <t>Lecture</t>
   </si>
@@ -171,6 +171,12 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Column1</t>
   </si>
 </sst>
 </file>
@@ -299,7 +305,20 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -441,20 +460,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G32" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G32"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="No" dataDxfId="6"/>
-    <tableColumn id="2" name="Lecture" dataDxfId="5"/>
-    <tableColumn id="3" name="Trainer" dataDxfId="4"/>
-    <tableColumn id="4" name="Date" dataDxfId="3"/>
-    <tableColumn id="5" name="Day of Week" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H32" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:H32"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="No" dataDxfId="7"/>
+    <tableColumn id="2" name="Lecture" dataDxfId="6"/>
+    <tableColumn id="3" name="Trainer" dataDxfId="5"/>
+    <tableColumn id="4" name="Date" dataDxfId="4"/>
+    <tableColumn id="5" name="Day of Week" dataDxfId="3">
       <calculatedColumnFormula>TEXT(Table1[[#This Row],[Date]],"dddd")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Time" dataDxfId="1"/>
-    <tableColumn id="7" name="Homework" dataDxfId="0">
+    <tableColumn id="6" name="Time" dataDxfId="2"/>
+    <tableColumn id="7" name="Homework" dataDxfId="1">
       <calculatedColumnFormula>Table1[[#This Row],[Date]]+7</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="8" name="Column1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -723,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -741,7 +761,7 @@
     <col min="8" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -763,8 +783,11 @@
       <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H1" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -788,7 +811,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -812,7 +835,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -837,7 +860,7 @@
         <v>42200</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -862,7 +885,7 @@
         <v>42201</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>3</v>
       </c>
@@ -887,7 +910,7 @@
         <v>42201</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>4</v>
       </c>
@@ -912,7 +935,7 @@
         <v>42205</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>4</v>
       </c>
@@ -937,7 +960,7 @@
         <v>42205</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>5</v>
       </c>
@@ -962,7 +985,7 @@
         <v>42207</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>5</v>
       </c>
@@ -987,7 +1010,7 @@
         <v>42207</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>6</v>
       </c>
@@ -1012,7 +1035,7 @@
         <v>42208</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>6</v>
       </c>
@@ -1037,7 +1060,7 @@
         <v>42208</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>7</v>
       </c>
@@ -1062,7 +1085,7 @@
         <v>42212</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>39</v>
       </c>
@@ -1085,8 +1108,9 @@
       <c r="G14" s="17" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>8</v>
       </c>
@@ -1111,7 +1135,7 @@
         <v>42214</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>8</v>
       </c>
@@ -1136,7 +1160,7 @@
         <v>42214</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>9</v>
       </c>
@@ -1161,7 +1185,7 @@
         <v>42215</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>9</v>
       </c>
@@ -1181,12 +1205,9 @@
       <c r="F18" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="8">
-        <f>Table1[[#This Row],[Date]]+7</f>
-        <v>42219</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>10</v>
       </c>
@@ -1211,55 +1232,58 @@
         <v>42219</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
+    <row r="20" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="12">
+      <c r="C20" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="17">
         <v>42213</v>
       </c>
-      <c r="E20" s="11" t="str">
+      <c r="E20" s="16" t="str">
         <f>TEXT(Table1[[#This Row],[Date]],"dddd")</f>
         <v>вторник</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="G20" s="17" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
+      <c r="H20" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
         <v>11</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="8">
         <v>42214</v>
       </c>
-      <c r="E21" s="2" t="str">
+      <c r="E21" s="7" t="str">
         <f>TEXT(Table1[[#This Row],[Date]],"dddd")</f>
         <v>сряда</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="13">
         <v>42214</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>12</v>
       </c>
@@ -1283,7 +1307,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>13</v>
       </c>
@@ -1307,7 +1331,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>39</v>
       </c>
@@ -1330,8 +1354,9 @@
       <c r="G24" s="12" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>14</v>
       </c>
@@ -1355,7 +1380,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>15</v>
       </c>
@@ -1380,7 +1405,7 @@
         <v>42236</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>16</v>
       </c>
@@ -1404,7 +1429,7 @@
         <v>42239</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>39</v>
       </c>
@@ -1428,8 +1453,9 @@
         <f>Table1[[#This Row],[Date]]+7</f>
         <v>42241</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>17</v>
       </c>
@@ -1453,7 +1479,7 @@
         <v>42235</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>18</v>
       </c>
@@ -1477,7 +1503,7 @@
         <v>42236</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>19</v>
       </c>
@@ -1501,7 +1527,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B32" s="4" t="s">
         <v>35</v>
       </c>

</xml_diff>